<commit_message>
fix: update gene regions according to mail Regions Data Tables Das hier ist die Region mit Deletionen, welche für BMPR1A relevant sind: hg 38 chr10:86756489-86768921 -> mit 2 kb links und rechts 16 kb (hg 38 chr10:86754489-86770921) anstatt von 121 kb (aktuelle Liste 10               86.755.013         86.876.083)
Das hier ist die 40 kb Region für GREM1-assoziierte CNVs basierend auf PMID: 22561515:
hg 38 chr15:32672738-32712558 (aktuell 400 kb im Design, 15 32.643.603               33.023.340)
</commit_message>
<xml_diff>
--- a/data/regions/regions_list.xlsx
+++ b/data/regions/regions_list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4452DF7-7E26-45DE-B2E3-35C714972952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A66AEF-3484-4741-BED7-131AE45FED08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C95C6FED-A9B1-47B9-B1E7-71E7CD4356DD}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C95C6FED-A9B1-47B9-B1E7-71E7CD4356DD}"/>
   </bookViews>
   <sheets>
     <sheet name="regions_cnvs" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>APC promoter, include all non coding exons (based on P043-E1 plus/minus 5kb)</t>
   </si>
   <si>
-    <t>GREM1 promoter (based on P378-D1 plus/minus 5kb)</t>
-  </si>
-  <si>
     <t>PTEN promoter (based on ME001-D1 plus/minus 5kb)</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>GREM1 promoter (based on PMID: 22561515)</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -529,13 +529,13 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -602,10 +602,10 @@
         <v>10</v>
       </c>
       <c r="I3" s="3">
-        <v>86755013</v>
+        <v>86754489</v>
       </c>
       <c r="J3" s="3">
-        <v>86876083</v>
+        <v>86770921</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>9</v>
@@ -637,13 +637,13 @@
         <v>15</v>
       </c>
       <c r="I4" s="3">
-        <v>32643603</v>
+        <v>32672738</v>
       </c>
       <c r="J4" s="3">
-        <v>33023340</v>
+        <v>32712558</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>87868674</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -783,7 +783,7 @@
         <v>7674064</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -800,13 +800,13 @@
         <v>32457087</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="3">
         <v>11</v>
@@ -818,7 +818,7 @@
         <v>32435552</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>